<commit_message>
refactor ADC reading logic
</commit_message>
<xml_diff>
--- a/design/NTC_calcs.xlsx
+++ b/design/NTC_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\bambu-chamber-heater\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EBA1A-3056-436C-B719-F3218E2F9F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3AF1F6-C035-4D8C-BDE4-71C46C862CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="2" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
+    <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{C15B9210-5287-4BB4-843A-B886E7D7C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart2" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Rref</t>
   </si>
@@ -129,16 +129,20 @@
   <si>
     <t>I (uA)</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,16 +158,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -171,11 +188,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -189,8 +222,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2236,10 +2274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3140C9DF-2692-47E8-B5FD-96C592C7023B}">
-  <dimension ref="B2:S34"/>
+  <dimension ref="B2:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2358,7 @@
       <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="12">
         <f>Vin*Rsensor/(Rsensor+Rref)</f>
         <v>2.7777777777777777</v>
       </c>
@@ -2332,12 +2370,36 @@
       <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="9">
         <f>Vout/Rsensor*1000</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="10">
+        <f>(Vin-Vout)/Rref</f>
+        <v>1.1111111111111109E-4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
+        <f>Vout/C17</f>
+        <v>25000.000000000004</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -2460,7 +2522,7 @@
         <v>327240</v>
       </c>
       <c r="E26" s="6">
-        <f>Vin/(Rref+D26)*1000</f>
+        <f t="shared" ref="E26:E33" si="0">Vin/(Rref+D26)*1000</f>
         <v>9.9415557028378621E-3</v>
       </c>
       <c r="F26" s="4">
@@ -2468,7 +2530,7 @@
         <v>9.9415557028378618</v>
       </c>
       <c r="G26" s="6">
-        <f>E26*D26/1000</f>
+        <f t="shared" ref="G26:G33" si="1">E26*D26/1000</f>
         <v>3.2532746881966617</v>
       </c>
     </row>
@@ -2480,15 +2542,15 @@
         <v>199990</v>
       </c>
       <c r="E27" s="6">
-        <f>Vin/(Rref+D27)*1000</f>
+        <f t="shared" si="0"/>
         <v>1.612194049538326E-2</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" ref="F27:F34" si="0">E27*1000</f>
+        <f t="shared" ref="F27:F33" si="2">E27*1000</f>
         <v>16.12194049538326</v>
       </c>
       <c r="G27" s="6">
-        <f>E27*D27/1000</f>
+        <f t="shared" si="1"/>
         <v>3.224226879671698</v>
       </c>
     </row>
@@ -2500,15 +2562,15 @@
         <v>100000</v>
       </c>
       <c r="E28" s="6">
-        <f>Vin/(Rref+D28)*1000</f>
+        <f t="shared" si="0"/>
         <v>3.151862464183381E-2</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.51862464183381</v>
       </c>
       <c r="G28" s="6">
-        <f>E28*D28/1000</f>
+        <f t="shared" si="1"/>
         <v>3.1518624641833815</v>
       </c>
     </row>
@@ -2520,15 +2582,15 @@
         <v>53500</v>
       </c>
       <c r="E29" s="6">
-        <f>Vin/(Rref+D29)*1000</f>
+        <f t="shared" si="0"/>
         <v>5.6701030927835044E-2</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>56.701030927835042</v>
       </c>
       <c r="G29" s="6">
-        <f>E29*D29/1000</f>
+        <f t="shared" si="1"/>
         <v>3.0335051546391751</v>
       </c>
     </row>
@@ -2540,15 +2602,15 @@
         <v>35899</v>
       </c>
       <c r="E30" s="6">
-        <f>Vin/(Rref+D30)*1000</f>
+        <f t="shared" si="0"/>
         <v>8.1282790216507791E-2</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>81.282790216507792</v>
       </c>
       <c r="G30" s="6">
-        <f>E30*D30/1000</f>
+        <f t="shared" si="1"/>
         <v>2.9179708859824132</v>
       </c>
     </row>
@@ -2560,15 +2622,15 @@
         <v>25000</v>
       </c>
       <c r="E31" s="6">
-        <f>Vin/(Rref+D31)*1000</f>
+        <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>111.1111111111111</v>
       </c>
       <c r="G31" s="6">
-        <f>E31*D31/1000</f>
+        <f t="shared" si="1"/>
         <v>2.7777777777777777</v>
       </c>
     </row>
@@ -2580,55 +2642,75 @@
         <v>12540</v>
       </c>
       <c r="E32" s="6">
-        <f>Vin/(Rref+D32)*1000</f>
+        <f t="shared" si="0"/>
         <v>0.19141531322505798</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>191.41531322505799</v>
       </c>
       <c r="G32" s="6">
-        <f>E32*D32/1000</f>
+        <f t="shared" si="1"/>
         <v>2.4003480278422269</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="D33" s="7">
-        <v>3340</v>
+        <v>6710</v>
       </c>
       <c r="E33" s="6">
-        <f>Vin/(Rref+D33)*1000</f>
-        <v>0.41044776119402981</v>
+        <f t="shared" si="0"/>
+        <v>0.2892199824715162</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="0"/>
-        <v>410.44776119402979</v>
+        <f t="shared" si="2"/>
+        <v>289.21998247151618</v>
       </c>
       <c r="G33" s="6">
-        <f>E33*D33/1000</f>
-        <v>1.3708955223880597</v>
+        <f t="shared" si="1"/>
+        <v>1.9406660823838737</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="D34" s="7">
-        <v>582</v>
+        <v>3340</v>
       </c>
       <c r="E34" s="6">
         <f>Vin/(Rref+D34)*1000</f>
-        <v>0.62476334721696325</v>
+        <v>0.41044776119402981</v>
       </c>
       <c r="F34" s="4">
-        <f t="shared" si="0"/>
-        <v>624.76334721696321</v>
+        <f>E34*1000</f>
+        <v>410.44776119402979</v>
       </c>
       <c r="G34" s="6">
         <f>E34*D34/1000</f>
+        <v>1.3708955223880597</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>200</v>
+      </c>
+      <c r="D35" s="7">
+        <v>582</v>
+      </c>
+      <c r="E35" s="6">
+        <f>Vin/(Rref+D35)*1000</f>
+        <v>0.62476334721696325</v>
+      </c>
+      <c r="F35" s="4">
+        <f>E35*1000</f>
+        <v>624.76334721696321</v>
+      </c>
+      <c r="G35" s="6">
+        <f>E35*D35/1000</f>
         <v>0.36361226808027258</v>
       </c>
     </row>

</xml_diff>